<commit_message>
upto stock still complete
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,52 +412,280 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H2"/>
+  <dimension ref="A2:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>fvs</t>
+          <t>a1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sv</t>
+          <t>noxo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sv</t>
+          <t>lipo+gino</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sv</t>
+          <t>23</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>12.3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>58</v>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>5555</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>246.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>noxo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>lipo+gino</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>12.9</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>5555</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>258.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>noxo</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>lipo+gino</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12.9</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>5555</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>167.70000000000002</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12.9</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>167.700</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>